<commit_message>
daily pattern stack view
</commit_message>
<xml_diff>
--- a/SlpGroupInfo.xlsx
+++ b/SlpGroupInfo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="544">
   <si>
     <t>SubjId</t>
   </si>
@@ -496,639 +496,6 @@
     <t>Owl</t>
   </si>
   <si>
-    <t>['caffeineD', 'sweetF', 'dairyP', 'grainP', 'eggP', 'vegetables', 'nutP', 'seafood', 'fruitP', 'meatP', 'compositeP', 'alcoholD', 'starchyP']</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 3, 3, 2, 0, 2, 0, 0, 0, 1, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 2, 0, 1, 0, 0, 1, 1, 0, 2, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 3, 2, 0, 1, 0, 0, 1, 0, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 2, 1, 1, 2, 0, 0, 0, 1, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 2, 0, 0, 0, 0, 0, 2, 1, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 4, 2, 0, 1, 0, 0, 2, 1, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 4, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[3, 2, 2, 2, 0, 0, 0, 0, 2, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 3, 2, 0, 1, 0, 0, 3, 3, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 2, 0, 1, 0, 1, 0, 1, 0, 3, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 3, 0, 1, 0, 0, 0, 1, 0, 1, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 2, 1, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 1, 0, 0, 2, 1, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[2, 1, 1, 0, 0, 1, 0, 1, 1, 0, 4, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 2, 0, 1, 0, 0, 0, 1, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 2, 0, 0, 0, 1, 0, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 0, 1, 0, 0, 0, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 3, 0, 1, 0, 0, 0, 0, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 3, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 3, 1, 0, 1, 0, 1, 1, 2, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 3, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 1, 0, 0, 0, 0, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 1, 0, 0, 0, 0, 2, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 4, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 1, 0, 0, 0, 3, 1, 4, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 2, 1, 1, 0, 0, 1, 1, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 1, 1, 0, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 0, 0, 0, 3, 2, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 1, 0, 1, 1, 1, 2, 0, 1, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 1, 0, 0, 0, 0, 1, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 1, 0, 0, 0, 2, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 1, 0, 0, 0, 0, 1, 0, 0, 3, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 4, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 4, 0, 1, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 1, 0, 2, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 2, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 2, 1, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 1, 2, 0, 0, 2, 0, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 2, 0, 4, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 1, 0, 0, 3, 1, 3, 1, 2]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 1, 0, 0, 3, 1, 3, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 1, 0, 0, 0, 2, 0, 2, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 2, 0, 0, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 1, 1]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[2, 4, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 3, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 1]</t>
-  </si>
-  <si>
-    <t>[1, 2, 1, 2, 0, 0, 0, 1, 2, 0, 0, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 2, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 0, 0, 0, 2, 2, 3, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 1, 0, 0, 0, 1, 2, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 1, 2, 0, 0, 0, 2, 0, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 4, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 1, 0, 0, 0, 0, 2, 0, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 3, 0, 0, 1, 0, 0, 0, 0, 4, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 3, 0, 0, 1, 1, 0, 0, 0, 0, 3, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 1, 0, 0, 1, 0, 0, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 0, 0, 2, 0, 0, 1, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 4, 0, 0, 0, 1, 0, 1, 0, 0, 3, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1]</t>
-  </si>
-  <si>
-    <t>[3, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[3, 3, 2, 2, 0, 0, 0, 0, 1, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 2, 2, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 2, 1, 0, 1, 0, 1, 1, 0, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 2, 2, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 2, 0, 0, 0, 0, 0, 0, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 2, 0, 1, 0, 0, 0, 0, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 1, 0, 2, 0, 0, 0, 1, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 2, 0, 0, 0, 0, 0, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 2, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 2, 0, 0, 0, 1, 3, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 3, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 2, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 1, 0, 0, 2, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 1, 0, 1, 0, 2, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 2, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 3, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 3, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 3, 0, 1, 0, 0, 2, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 0, 0, 0, 1, 2, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 2, 0, 0, 0, 1, 4, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 0, 0, 0, 0, 3, 0, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 2, 0, 0, 0, 0, 0, 0, 4, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 0, 1, 1, 0, 0, 2, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 2, 0, 3, 0, 0, 1, 0, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 0, 1, 0, 0, 2, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 1, 0, 0, 1, 2, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 4, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 2, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 3, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 2, 0, 1, 0, 0, 0, 0, 1, 1, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 0, 0, 0, 0, 0, 0, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 1, 2, 0, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 2, 1, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 3, 2, 0, 1, 1, 0, 1, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[2, 1, 2, 2, 0, 2, 2, 0, 2, 0, 3, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 3, 1, 0, 2, 0, 1, 2, 0, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 3, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 1, 0, 0, 1, 0, 2, 0, 4, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 2, 0, 1, 0, 0, 0, 0, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 1, 2, 0, 2, 1, 1, 1, 0, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 3, 0, 1, 1, 0, 3, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 2, 0, 1, 0, 0, 1, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 2, 0, 1, 0, 0, 1, 0, 2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 3, 0, 1, 1, 0, 1, 0, 2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 3, 1, 3, 0, 1, 1, 0, 2, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 3, 1, 0, 1, 1, 0, 1, 0, 5, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 1, 1, 1, 1, 0, 0, 2, 2, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 1, 0, 0, 3, 0, 2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 1, 0, 1, 0, 0, 2, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 1, 0, 0, 3, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 2, 2, 0]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 1, 0, 1, 0, 0, 2, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0, 1, 0, 1, 0, 0, 2, 0, 1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0]</t>
-  </si>
-  <si>
     <t>[0, 1, 0, 0, 5, 0, 2, 2]</t>
   </si>
   <si>
@@ -1654,8 +1021,637 @@
     <t>[0, 4, 0, 0, 1, 0, 0, 2]</t>
   </si>
   <si>
-    <t>['caffeineD', 'sweetF', 'dairyP', 'grainP', 'eggP', 'vegetables', 'nutP', 'seafood', 'fruitP', 'meatP', 'compositeP', 'alcoholD', 'starchyP']</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>['caffeineD', 'snack', 'dairyP', 'grainP', 'eggP', 'alcoholD', 'seafood', 'fruitP', 'meatP', 'compositeP', 'vegetables', 'starchyP']</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 2, 0]</t>
+  </si>
+  <si>
+    <t>[1, 3, 3, 2, 0, 0, 0, 0, 1, 0, 2, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 2, 0, 2, 0, 1, 1, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 3, 2, 0, 1, 0, 1, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 1, 1, 1, 0, 0, 1, 1, 2, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 0, 0, 0, 0, 2, 1, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 4, 2, 0, 0, 0, 2, 1, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 1, 0, 0, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 0, 0, 0, 4, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 0, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 3, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 0, 0, 0, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 0, 0, 0, 2, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[3, 2, 2, 2, 0, 0, 0, 2, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 3, 2, 0, 0, 0, 3, 3, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 2, 0, 1, 0, 0, 1, 0, 3, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 0, 0, 0, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 3, 0, 1, 0, 0, 1, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 2, 1, 2, 0, 0, 0, 0, 0, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 2, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[2, 1, 1, 0, 0, 0, 1, 1, 0, 4, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 0, 0, 1, 0, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 2, 0, 0, 0, 0, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 2, 0, 0, 0, 0, 1, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 2, 0, 0, 1, 0, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 2, 0, 0, 0, 0, 1, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 3, 0, 0, 0, 0, 0, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 1, 0, 1, 0, 1, 1, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 3, 1, 0, 0, 1, 1, 2, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 0, 0, 2, 3, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 0, 0, 0, 2, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 1, 0, 0, 0, 0, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 1, 0, 0, 0, 2, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 0, 1, 1, 4, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 1, 0, 0, 3, 1, 4, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 0, 0, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 2, 1, 0, 0, 1, 1, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 0, 0, 1, 0, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 0, 0, 0, 0, 0, 0, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 3, 0, 0, 0, 0, 0, 0, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 0, 0, 3, 2, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 3, 0, 1, 0, 0, 1, 2, 0, 1, 1, 2]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 1, 0, 0, 0, 1, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 0, 0, 0, 2, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 0, 0, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 1, 0, 0, 0, 1, 0, 0, 3, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 0, 1, 4, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 4, 0, 0, 0, 0, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 1, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 1, 0, 0, 0, 2, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 2, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 0, 2, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 1, 1, 0, 2, 0, 1, 2, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 2, 0, 4, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 1, 0, 3, 1, 3, 1, 2]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 3, 1, 3, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 1, 0, 2, 0, 2, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 1, 0, 2, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 0, 1, 1, 2, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[2, 4, 0, 0, 0, 0, 0, 1, 1, 0, 0, 2]</t>
+  </si>
+  <si>
+    <t>[0, 3, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 2]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 2]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 2, 0, 1, 0, 0, 0, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 2, 1, 2, 0, 1, 1, 2, 0, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 2, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 2, 2, 3, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 0, 0, 1, 2, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 1, 0, 1, 1, 0, 2]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 0, 0, 0, 2, 0, 2, 2]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 1, 0, 0, 0, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 1, 0, 0, 0, 0, 4, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 1, 0, 0, 0, 2, 0, 0, 2]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 1, 0, 0, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 3, 0, 0, 0, 0, 0, 0, 4, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 3, 0, 0, 1, 0, 0, 0, 0, 3, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 0, 0, 0, 0, 1, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 0, 1, 0, 1, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 1, 0, 0, 0, 0, 0, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 0, 0, 0, 0, 1, 0, 2, 2, 0]</t>
+  </si>
+  <si>
+    <t>[0, 4, 0, 0, 0, 1, 1, 0, 0, 3, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[3, 2, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[3, 3, 2, 2, 0, 0, 0, 1, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 0, 0, 2, 0, 1, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 0, 2, 1, 0, 0, 1, 1, 0, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 2, 2, 1, 0, 1, 0, 0, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 2, 0, 1, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 2, 0, 0, 0, 0, 0, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 1, 0, 0, 0, 0, 1, 3, 2, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 2, 0, 0, 0, 0, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 0, 1, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 1, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 0, 0, 1, 3, 2, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 0, 1, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 3, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 0, 1, 2, 0, 1, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 0, 0, 0, 0, 2, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 1, 0, 0, 0, 0, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 0, 2, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 1, 0, 0, 2, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 3, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 2, 0, 0, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 1, 3, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 0, 0, 0, 0, 0, 1, 3, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 1, 1, 3, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 1, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 1, 1, 3, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 3, 0, 0, 0, 2, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 0, 0, 1, 2, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 2, 0, 0, 1, 4, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 0, 1, 0, 3, 0, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 2, 0, 0, 0, 0, 0, 4, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 0, 1, 0, 0, 2, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 2, 2, 0, 1, 0, 1, 0, 1, 3, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 1, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 0, 0, 0, 2, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 1, 2, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 1, 0, 1, 0, 4, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 1, 0, 0, 0, 2, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 2, 0, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 1, 0, 0, 1, 3, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 2, 0, 1, 0, 0, 0, 1, 1, 2, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 2, 0, 1, 0, 0, 0, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 1, 2, 0, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 1, 0, 2, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 0, 0, 0, 0, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 2, 0, 0, 0, 1, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[2, 3, 2, 2, 0, 0, 0, 2, 0, 3, 2, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 3, 1, 0, 0, 1, 2, 0, 1, 2, 1]</t>
+  </si>
+  <si>
+    <t>[0, 3, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 2, 1, 0, 0, 0, 2, 0, 4, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 2, 0, 0, 0, 0, 0, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 3, 1, 2, 0, 0, 1, 1, 0, 0, 2, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 1, 3, 0, 0, 0, 3, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 2, 0, 0, 0, 1, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 2, 0, 0, 0, 1, 0, 2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 2, 1, 3, 0, 1, 0, 1, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 4, 1, 3, 0, 0, 0, 2, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 3, 3, 1, 0, 0, 0, 1, 0, 5, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 1, 1, 1, 0, 0, 2, 2, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 3, 0, 2, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 1, 0, 0, 0, 2, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 3, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 2, 0, 0, 1, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 1, 0, 0, 0, 2, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 1, 0, 1, 0, 0, 0, 2, 0, 1, 1, 0]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0]</t>
   </si>
 </sst>
 </file>
@@ -1862,11 +1858,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2127879288"/>
-        <c:axId val="2129171960"/>
+        <c:axId val="-2120493064"/>
+        <c:axId val="-2120639784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127879288"/>
+        <c:axId val="-2120493064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1905,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2129171960"/>
+        <c:crossAx val="-2120639784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1917,7 +1913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2129171960"/>
+        <c:axId val="-2120639784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,7 +1964,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127879288"/>
+        <c:crossAx val="-2120493064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2885,15 +2881,15 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="83.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="97.1640625" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="93.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2948,10 +2944,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>159</v>
+        <v>334</v>
       </c>
       <c r="G2" s="1">
         <v>7.5211110000000003</v>
@@ -2987,10 +2983,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>160</v>
+        <v>335</v>
       </c>
       <c r="G3" s="1">
         <v>7.71</v>
@@ -3026,10 +3022,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>161</v>
+        <v>336</v>
       </c>
       <c r="G4" s="1">
         <v>10.491111</v>
@@ -3062,13 +3058,13 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>369</v>
+        <v>158</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>544</v>
+        <v>333</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>162</v>
+        <v>337</v>
       </c>
       <c r="G5" s="1">
         <v>8.2922220000000006</v>
@@ -3101,13 +3097,13 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>370</v>
+        <v>159</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>163</v>
+        <v>338</v>
       </c>
       <c r="G6" s="1">
         <v>7.8766670000000003</v>
@@ -3140,13 +3136,13 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>371</v>
+        <v>160</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>164</v>
+        <v>339</v>
       </c>
       <c r="G7" s="1">
         <v>7.2411110000000001</v>
@@ -3179,13 +3175,13 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>372</v>
+        <v>161</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>165</v>
+        <v>340</v>
       </c>
       <c r="G8" s="1">
         <v>7.951111</v>
@@ -3218,13 +3214,13 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>373</v>
+        <v>162</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>166</v>
+        <v>341</v>
       </c>
       <c r="G9" s="1">
         <v>7.1366670000000001</v>
@@ -3257,13 +3253,13 @@
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>374</v>
+        <v>163</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>167</v>
+        <v>342</v>
       </c>
       <c r="G10" s="1">
         <v>6.9388889999999996</v>
@@ -3296,13 +3292,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>375</v>
+        <v>164</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>168</v>
+        <v>343</v>
       </c>
       <c r="G11" s="1">
         <v>8.3233329999999999</v>
@@ -3335,13 +3331,13 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>376</v>
+        <v>165</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>169</v>
+        <v>344</v>
       </c>
       <c r="G12" s="1">
         <v>8.4077780000000004</v>
@@ -3374,13 +3370,13 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>377</v>
+        <v>166</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>170</v>
+        <v>345</v>
       </c>
       <c r="G13" s="1">
         <v>7.8533330000000001</v>
@@ -3416,10 +3412,10 @@
         <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>171</v>
+        <v>346</v>
       </c>
       <c r="G14" s="1">
         <v>9.9488889999999994</v>
@@ -3455,10 +3451,10 @@
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>172</v>
+        <v>347</v>
       </c>
       <c r="G15" s="1">
         <v>8.9911110000000001</v>
@@ -3491,13 +3487,13 @@
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>378</v>
+        <v>167</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>173</v>
+        <v>348</v>
       </c>
       <c r="G16" s="1">
         <v>12.334444</v>
@@ -3530,13 +3526,13 @@
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>379</v>
+        <v>168</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>174</v>
+        <v>349</v>
       </c>
       <c r="G17" s="1">
         <v>12.095556</v>
@@ -3569,13 +3565,13 @@
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>380</v>
+        <v>169</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>175</v>
+        <v>350</v>
       </c>
       <c r="G18" s="1">
         <v>9.7555560000000003</v>
@@ -3608,13 +3604,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>381</v>
+        <v>170</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>176</v>
+        <v>351</v>
       </c>
       <c r="G19" s="1">
         <v>10.98</v>
@@ -3647,13 +3643,13 @@
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>382</v>
+        <v>171</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>177</v>
+        <v>352</v>
       </c>
       <c r="G20" s="1">
         <v>8.9600000000000009</v>
@@ -3686,13 +3682,13 @@
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>383</v>
+        <v>172</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>178</v>
+        <v>353</v>
       </c>
       <c r="G21" s="1">
         <v>7.7511109999999999</v>
@@ -3725,13 +3721,13 @@
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>384</v>
+        <v>173</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>179</v>
+        <v>354</v>
       </c>
       <c r="G22" s="1">
         <v>11.011111</v>
@@ -3764,13 +3760,13 @@
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>385</v>
+        <v>174</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>180</v>
+        <v>355</v>
       </c>
       <c r="G23" s="1">
         <v>8.2722219999999993</v>
@@ -3803,13 +3799,13 @@
         <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>380</v>
+        <v>169</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>181</v>
+        <v>356</v>
       </c>
       <c r="G24" s="1">
         <v>8.5844439999999995</v>
@@ -3842,13 +3838,13 @@
         <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>386</v>
+        <v>175</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>182</v>
+        <v>357</v>
       </c>
       <c r="G25" s="1">
         <v>8.4911110000000001</v>
@@ -3881,13 +3877,13 @@
         <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>387</v>
+        <v>176</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>183</v>
+        <v>358</v>
       </c>
       <c r="G26" s="1">
         <v>8.6788889999999999</v>
@@ -3920,13 +3916,13 @@
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>388</v>
+        <v>177</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>184</v>
+        <v>359</v>
       </c>
       <c r="G27" s="1">
         <v>9.4811110000000003</v>
@@ -3962,10 +3958,10 @@
         <v>41</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="G28" s="1">
         <v>8.9388889999999996</v>
@@ -3998,13 +3994,13 @@
         <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>389</v>
+        <v>178</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>186</v>
+        <v>361</v>
       </c>
       <c r="G29" s="1">
         <v>8.1366669999999992</v>
@@ -4037,13 +4033,13 @@
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>390</v>
+        <v>179</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>187</v>
+        <v>362</v>
       </c>
       <c r="G30" s="1">
         <v>8.6266669999999994</v>
@@ -4076,13 +4072,13 @@
         <v>6</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>391</v>
+        <v>180</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>188</v>
+        <v>363</v>
       </c>
       <c r="G31" s="1">
         <v>8.7100000000000009</v>
@@ -4115,13 +4111,13 @@
         <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>391</v>
+        <v>180</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>189</v>
+        <v>364</v>
       </c>
       <c r="G32" s="1">
         <v>7.97</v>
@@ -4154,13 +4150,13 @@
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>392</v>
+        <v>181</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>190</v>
+        <v>365</v>
       </c>
       <c r="G33" s="1">
         <v>7.4844439999999999</v>
@@ -4193,13 +4189,13 @@
         <v>6</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>393</v>
+        <v>182</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>191</v>
+        <v>366</v>
       </c>
       <c r="G34" s="1">
         <v>8.7411110000000001</v>
@@ -4232,13 +4228,13 @@
         <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>394</v>
+        <v>183</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>192</v>
+        <v>367</v>
       </c>
       <c r="G35" s="1">
         <v>8.5422220000000006</v>
@@ -4271,13 +4267,13 @@
         <v>6</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>395</v>
+        <v>184</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>193</v>
+        <v>368</v>
       </c>
       <c r="G36" s="1">
         <v>9.1155559999999998</v>
@@ -4310,13 +4306,13 @@
         <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>396</v>
+        <v>185</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>194</v>
+        <v>369</v>
       </c>
       <c r="G37" s="1">
         <v>9.5011109999999999</v>
@@ -4349,13 +4345,13 @@
         <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>397</v>
+        <v>186</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>195</v>
+        <v>370</v>
       </c>
       <c r="G38" s="1">
         <v>8.0533330000000003</v>
@@ -4391,10 +4387,10 @@
         <v>49</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>196</v>
+        <v>371</v>
       </c>
       <c r="G39" s="1">
         <v>8.0111109999999996</v>
@@ -4430,10 +4426,10 @@
         <v>50</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>197</v>
+        <v>372</v>
       </c>
       <c r="G40" s="1">
         <v>7.0333329999999998</v>
@@ -4466,13 +4462,13 @@
         <v>6</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>398</v>
+        <v>187</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>198</v>
+        <v>373</v>
       </c>
       <c r="G41" s="1">
         <v>10.282222000000001</v>
@@ -4505,13 +4501,13 @@
         <v>6</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>399</v>
+        <v>188</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>199</v>
+        <v>374</v>
       </c>
       <c r="G42" s="1">
         <v>7.83</v>
@@ -4544,13 +4540,13 @@
         <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>400</v>
+        <v>189</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>200</v>
+        <v>375</v>
       </c>
       <c r="G43" s="1">
         <v>5.8233329999999999</v>
@@ -4586,10 +4582,10 @@
         <v>51</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>201</v>
+        <v>376</v>
       </c>
       <c r="G44" s="1">
         <v>9.0322220000000009</v>
@@ -4622,13 +4618,13 @@
         <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>401</v>
+        <v>190</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>202</v>
+        <v>377</v>
       </c>
       <c r="G45" s="1">
         <v>8.0011109999999999</v>
@@ -4661,13 +4657,13 @@
         <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>402</v>
+        <v>191</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>203</v>
+        <v>378</v>
       </c>
       <c r="G46" s="1">
         <v>9.3144439999999999</v>
@@ -4700,13 +4696,13 @@
         <v>6</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>403</v>
+        <v>192</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>204</v>
+        <v>379</v>
       </c>
       <c r="G47" s="1">
         <v>8.6988889999999994</v>
@@ -4742,10 +4738,10 @@
         <v>67</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>205</v>
+        <v>380</v>
       </c>
       <c r="G48" s="1">
         <v>9.0844439999999995</v>
@@ -4778,13 +4774,13 @@
         <v>6</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>404</v>
+        <v>193</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>206</v>
+        <v>381</v>
       </c>
       <c r="G49" s="1">
         <v>10.981111</v>
@@ -4817,13 +4813,13 @@
         <v>6</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>405</v>
+        <v>194</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>207</v>
+        <v>382</v>
       </c>
       <c r="G50" s="1">
         <v>8.3755559999999996</v>
@@ -4856,13 +4852,13 @@
         <v>6</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>406</v>
+        <v>195</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>208</v>
+        <v>383</v>
       </c>
       <c r="G51" s="1">
         <v>6.47</v>
@@ -4895,13 +4891,13 @@
         <v>6</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>407</v>
+        <v>196</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>209</v>
+        <v>384</v>
       </c>
       <c r="G52" s="1">
         <v>8.1577780000000004</v>
@@ -4934,13 +4930,13 @@
         <v>6</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>408</v>
+        <v>197</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>210</v>
+        <v>385</v>
       </c>
       <c r="G53" s="1">
         <v>11.015556</v>
@@ -4976,10 +4972,10 @@
         <v>58</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>211</v>
+        <v>386</v>
       </c>
       <c r="G54" s="1">
         <v>9.3866669999999992</v>
@@ -5012,13 +5008,13 @@
         <v>6</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>409</v>
+        <v>198</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>212</v>
+        <v>387</v>
       </c>
       <c r="G55" s="1">
         <v>8.2511109999999999</v>
@@ -5051,13 +5047,13 @@
         <v>6</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>410</v>
+        <v>199</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>213</v>
+        <v>388</v>
       </c>
       <c r="G56" s="1">
         <v>10.584444</v>
@@ -5090,13 +5086,13 @@
         <v>6</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>411</v>
+        <v>200</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>214</v>
+        <v>389</v>
       </c>
       <c r="G57" s="1">
         <v>9.2922220000000006</v>
@@ -5129,13 +5125,13 @@
         <v>6</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>412</v>
+        <v>201</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>215</v>
+        <v>390</v>
       </c>
       <c r="G58" s="1">
         <v>9.0111109999999996</v>
@@ -5168,13 +5164,13 @@
         <v>6</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>413</v>
+        <v>202</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>216</v>
+        <v>391</v>
       </c>
       <c r="G59" s="1">
         <v>8.3133330000000001</v>
@@ -5207,13 +5203,13 @@
         <v>6</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>414</v>
+        <v>203</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>217</v>
+        <v>392</v>
       </c>
       <c r="G60" s="1">
         <v>7.6466669999999999</v>
@@ -5246,13 +5242,13 @@
         <v>6</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>415</v>
+        <v>204</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>218</v>
+        <v>393</v>
       </c>
       <c r="G61" s="1">
         <v>5.355556</v>
@@ -5288,10 +5284,10 @@
         <v>67</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>219</v>
+        <v>394</v>
       </c>
       <c r="G62" s="1">
         <v>7.6977779999999996</v>
@@ -5327,10 +5323,10 @@
         <v>69</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>220</v>
+        <v>395</v>
       </c>
       <c r="G63" s="1">
         <v>7.1566669999999997</v>
@@ -5363,13 +5359,13 @@
         <v>6</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>416</v>
+        <v>205</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>170</v>
+        <v>345</v>
       </c>
       <c r="G64" s="1">
         <v>8.2822220000000009</v>
@@ -5402,13 +5398,13 @@
         <v>6</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>417</v>
+        <v>206</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>221</v>
+        <v>396</v>
       </c>
       <c r="G65" s="1">
         <v>6.927778</v>
@@ -5441,13 +5437,13 @@
         <v>6</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>418</v>
+        <v>207</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>222</v>
+        <v>397</v>
       </c>
       <c r="G66" s="1">
         <v>7.7077780000000002</v>
@@ -5480,13 +5476,13 @@
         <v>6</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>419</v>
+        <v>208</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>223</v>
+        <v>398</v>
       </c>
       <c r="G67" s="1">
         <v>7.2722220000000002</v>
@@ -5519,13 +5515,13 @@
         <v>6</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>420</v>
+        <v>209</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>224</v>
+        <v>399</v>
       </c>
       <c r="G68" s="1">
         <v>10.220000000000001</v>
@@ -5558,13 +5554,13 @@
         <v>6</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>421</v>
+        <v>210</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>225</v>
+        <v>400</v>
       </c>
       <c r="G69" s="1">
         <v>8.1877779999999998</v>
@@ -5597,13 +5593,13 @@
         <v>6</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>422</v>
+        <v>211</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>226</v>
+        <v>401</v>
       </c>
       <c r="G70" s="1">
         <v>6.855556</v>
@@ -5636,13 +5632,13 @@
         <v>6</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>423</v>
+        <v>212</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>227</v>
+        <v>402</v>
       </c>
       <c r="G71" s="1">
         <v>8.3455560000000002</v>
@@ -5678,10 +5674,10 @@
         <v>80</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>228</v>
+        <v>403</v>
       </c>
       <c r="G72" s="1">
         <v>8.6577780000000004</v>
@@ -5714,13 +5710,13 @@
         <v>6</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>424</v>
+        <v>213</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>229</v>
+        <v>404</v>
       </c>
       <c r="G73" s="1">
         <v>9.2200000000000006</v>
@@ -5753,13 +5749,13 @@
         <v>6</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>425</v>
+        <v>214</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>230</v>
+        <v>405</v>
       </c>
       <c r="G74" s="1">
         <v>8.5533330000000003</v>
@@ -5792,13 +5788,13 @@
         <v>6</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>426</v>
+        <v>215</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>231</v>
+        <v>406</v>
       </c>
       <c r="G75" s="1">
         <v>8.0222219999999993</v>
@@ -5831,13 +5827,13 @@
         <v>6</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>427</v>
+        <v>216</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>232</v>
+        <v>407</v>
       </c>
       <c r="G76" s="1">
         <v>10.605556</v>
@@ -5870,13 +5866,13 @@
         <v>6</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>428</v>
+        <v>217</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>233</v>
+        <v>408</v>
       </c>
       <c r="G77" s="1">
         <v>9.0322220000000009</v>
@@ -5909,13 +5905,13 @@
         <v>6</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>429</v>
+        <v>218</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>196</v>
+        <v>371</v>
       </c>
       <c r="G78" s="1">
         <v>7.94</v>
@@ -5948,13 +5944,13 @@
         <v>6</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>430</v>
+        <v>219</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>234</v>
+        <v>409</v>
       </c>
       <c r="G79" s="1">
         <v>7.7611109999999996</v>
@@ -5987,13 +5983,13 @@
         <v>6</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>431</v>
+        <v>220</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>166</v>
+        <v>341</v>
       </c>
       <c r="G80" s="1">
         <v>7.8766670000000003</v>
@@ -6026,13 +6022,13 @@
         <v>6</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>432</v>
+        <v>221</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>235</v>
+        <v>410</v>
       </c>
       <c r="G81" s="1">
         <v>8.5633330000000001</v>
@@ -6065,13 +6061,13 @@
         <v>6</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>433</v>
+        <v>222</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>236</v>
+        <v>411</v>
       </c>
       <c r="G82" s="1">
         <v>7.1888889999999996</v>
@@ -6104,13 +6100,13 @@
         <v>6</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>434</v>
+        <v>223</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>237</v>
+        <v>412</v>
       </c>
       <c r="G83" s="1">
         <v>7.9488890000000003</v>
@@ -6143,13 +6139,13 @@
         <v>6</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>435</v>
+        <v>224</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>238</v>
+        <v>413</v>
       </c>
       <c r="G84" s="1">
         <v>7.1577780000000004</v>
@@ -6182,13 +6178,13 @@
         <v>6</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>436</v>
+        <v>225</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>239</v>
+        <v>414</v>
       </c>
       <c r="G85" s="1">
         <v>8.8655559999999998</v>
@@ -6224,10 +6220,10 @@
         <v>86</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>240</v>
+        <v>415</v>
       </c>
       <c r="G86" s="1">
         <v>9.3033330000000003</v>
@@ -6263,10 +6259,10 @@
         <v>88</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>241</v>
+        <v>416</v>
       </c>
       <c r="G87" s="1">
         <v>7.2922219999999998</v>
@@ -6299,13 +6295,13 @@
         <v>6</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>437</v>
+        <v>226</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>242</v>
+        <v>417</v>
       </c>
       <c r="G88" s="1">
         <v>5.5744439999999997</v>
@@ -6341,10 +6337,10 @@
         <v>23</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>243</v>
+        <v>418</v>
       </c>
       <c r="G89" s="1">
         <v>7.2922219999999998</v>
@@ -6377,13 +6373,13 @@
         <v>6</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>438</v>
+        <v>227</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>244</v>
+        <v>419</v>
       </c>
       <c r="G90" s="1">
         <v>7.4388889999999996</v>
@@ -6416,13 +6412,13 @@
         <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>439</v>
+        <v>228</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>245</v>
+        <v>420</v>
       </c>
       <c r="G91" s="1">
         <v>7.6988890000000003</v>
@@ -6455,13 +6451,13 @@
         <v>6</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>440</v>
+        <v>229</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>246</v>
+        <v>421</v>
       </c>
       <c r="G92" s="1">
         <v>7.7722220000000002</v>
@@ -6494,13 +6490,13 @@
         <v>6</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>441</v>
+        <v>230</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>247</v>
+        <v>422</v>
       </c>
       <c r="G93" s="1">
         <v>8.1155559999999998</v>
@@ -6533,13 +6529,13 @@
         <v>6</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>442</v>
+        <v>231</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>248</v>
+        <v>423</v>
       </c>
       <c r="G94" s="1">
         <v>7.1255559999999996</v>
@@ -6572,13 +6568,13 @@
         <v>6</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>443</v>
+        <v>232</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>249</v>
+        <v>424</v>
       </c>
       <c r="G95" s="1">
         <v>7.72</v>
@@ -6611,13 +6607,13 @@
         <v>6</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>444</v>
+        <v>233</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>250</v>
+        <v>425</v>
       </c>
       <c r="G96" s="1">
         <v>8.3444439999999993</v>
@@ -6653,10 +6649,10 @@
         <v>91</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>251</v>
+        <v>426</v>
       </c>
       <c r="G97" s="1">
         <v>9.3444439999999993</v>
@@ -6692,10 +6688,10 @@
         <v>92</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>252</v>
+        <v>427</v>
       </c>
       <c r="G98" s="1">
         <v>9.0111109999999996</v>
@@ -6731,10 +6727,10 @@
         <v>69</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>253</v>
+        <v>428</v>
       </c>
       <c r="G99" s="1">
         <v>8.5955560000000002</v>
@@ -6767,13 +6763,13 @@
         <v>6</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>445</v>
+        <v>234</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>254</v>
+        <v>429</v>
       </c>
       <c r="G100" s="1">
         <v>10.001111</v>
@@ -6806,13 +6802,13 @@
         <v>6</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>446</v>
+        <v>235</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>255</v>
+        <v>430</v>
       </c>
       <c r="G101" s="1">
         <v>7.8866670000000001</v>
@@ -6845,13 +6841,13 @@
         <v>6</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>378</v>
+        <v>167</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>256</v>
+        <v>431</v>
       </c>
       <c r="G102" s="1">
         <v>6.7511109999999999</v>
@@ -6884,13 +6880,13 @@
         <v>6</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>447</v>
+        <v>236</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>257</v>
+        <v>432</v>
       </c>
       <c r="G103" s="1">
         <v>8.0222219999999993</v>
@@ -6923,13 +6919,13 @@
         <v>6</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>448</v>
+        <v>237</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>258</v>
+        <v>433</v>
       </c>
       <c r="G104" s="1">
         <v>5.782222</v>
@@ -6962,13 +6958,13 @@
         <v>6</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>449</v>
+        <v>238</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>259</v>
+        <v>434</v>
       </c>
       <c r="G105" s="1">
         <v>8.1155559999999998</v>
@@ -7001,13 +6997,13 @@
         <v>6</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>450</v>
+        <v>239</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>260</v>
+        <v>435</v>
       </c>
       <c r="G106" s="1">
         <v>8.427778</v>
@@ -7040,13 +7036,13 @@
         <v>6</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>451</v>
+        <v>240</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>261</v>
+        <v>436</v>
       </c>
       <c r="G107" s="1">
         <v>7.927778</v>
@@ -7079,13 +7075,13 @@
         <v>6</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>452</v>
+        <v>241</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>262</v>
+        <v>437</v>
       </c>
       <c r="G108" s="1">
         <v>8.5744439999999997</v>
@@ -7118,13 +7114,13 @@
         <v>6</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>453</v>
+        <v>242</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>263</v>
+        <v>438</v>
       </c>
       <c r="G109" s="1">
         <v>8.5955560000000002</v>
@@ -7157,13 +7153,13 @@
         <v>6</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>454</v>
+        <v>243</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>264</v>
+        <v>439</v>
       </c>
       <c r="G110" s="1">
         <v>6.9188890000000001</v>
@@ -7199,10 +7195,10 @@
         <v>94</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>265</v>
+        <v>440</v>
       </c>
       <c r="G111" s="1">
         <v>9.6466670000000008</v>
@@ -7238,10 +7234,10 @@
         <v>95</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>266</v>
+        <v>441</v>
       </c>
       <c r="G112" s="1">
         <v>7.7611109999999996</v>
@@ -7277,10 +7273,10 @@
         <v>96</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>267</v>
+        <v>442</v>
       </c>
       <c r="G113" s="1">
         <v>6.7511109999999999</v>
@@ -7313,13 +7309,13 @@
         <v>6</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>455</v>
+        <v>244</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>268</v>
+        <v>443</v>
       </c>
       <c r="G114" s="1">
         <v>6.3444440000000002</v>
@@ -7352,13 +7348,13 @@
         <v>6</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>456</v>
+        <v>245</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>269</v>
+        <v>444</v>
       </c>
       <c r="G115" s="1">
         <v>8.3866669999999992</v>
@@ -7391,13 +7387,13 @@
         <v>6</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>457</v>
+        <v>246</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>270</v>
+        <v>445</v>
       </c>
       <c r="G116" s="1">
         <v>6.81</v>
@@ -7430,13 +7426,13 @@
         <v>6</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>458</v>
+        <v>247</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>271</v>
+        <v>446</v>
       </c>
       <c r="G117" s="1">
         <v>8.2511109999999999</v>
@@ -7469,13 +7465,13 @@
         <v>6</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>459</v>
+        <v>248</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>272</v>
+        <v>447</v>
       </c>
       <c r="G118" s="1">
         <v>9.3977780000000006</v>
@@ -7508,13 +7504,13 @@
         <v>6</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>460</v>
+        <v>249</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>273</v>
+        <v>448</v>
       </c>
       <c r="G119" s="1">
         <v>7.22</v>
@@ -7547,13 +7543,13 @@
         <v>6</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>461</v>
+        <v>250</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>274</v>
+        <v>449</v>
       </c>
       <c r="G120" s="1">
         <v>6.1466669999999999</v>
@@ -7586,13 +7582,13 @@
         <v>6</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>462</v>
+        <v>251</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>275</v>
+        <v>450</v>
       </c>
       <c r="G121" s="1">
         <v>13.156667000000001</v>
@@ -7625,13 +7621,13 @@
         <v>6</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>463</v>
+        <v>252</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>276</v>
+        <v>451</v>
       </c>
       <c r="G122" s="1">
         <v>9.9177780000000002</v>
@@ -7664,13 +7660,13 @@
         <v>6</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>464</v>
+        <v>253</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
       <c r="G123" s="1">
         <v>7.1877779999999998</v>
@@ -7706,10 +7702,10 @@
         <v>98</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>278</v>
+        <v>453</v>
       </c>
       <c r="G124" s="1">
         <v>8.9377779999999998</v>
@@ -7742,13 +7738,13 @@
         <v>6</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>465</v>
+        <v>254</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>279</v>
+        <v>454</v>
       </c>
       <c r="G125" s="1">
         <v>8.4700000000000006</v>
@@ -7781,13 +7777,13 @@
         <v>6</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>466</v>
+        <v>255</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>280</v>
+        <v>455</v>
       </c>
       <c r="G126" s="1">
         <v>9.2922220000000006</v>
@@ -7820,13 +7816,13 @@
         <v>6</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>467</v>
+        <v>256</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>281</v>
+        <v>456</v>
       </c>
       <c r="G127" s="1">
         <v>7.8133330000000001</v>
@@ -7859,13 +7855,13 @@
         <v>6</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>468</v>
+        <v>257</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>282</v>
+        <v>457</v>
       </c>
       <c r="G128" s="1">
         <v>8.6366669999999992</v>
@@ -7898,13 +7894,13 @@
         <v>6</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>469</v>
+        <v>258</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>283</v>
+        <v>458</v>
       </c>
       <c r="G129" s="1">
         <v>8.8344439999999995</v>
@@ -7940,10 +7936,10 @@
         <v>101</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>284</v>
+        <v>459</v>
       </c>
       <c r="G130" s="1">
         <v>7.9755560000000001</v>
@@ -7976,13 +7972,13 @@
         <v>6</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>470</v>
+        <v>259</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>285</v>
+        <v>460</v>
       </c>
       <c r="G131" s="1">
         <v>8.2622219999999995</v>
@@ -8015,13 +8011,13 @@
         <v>6</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>471</v>
+        <v>260</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>286</v>
+        <v>461</v>
       </c>
       <c r="G132" s="1">
         <v>7.1155559999999998</v>
@@ -8057,10 +8053,10 @@
         <v>104</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>287</v>
+        <v>462</v>
       </c>
       <c r="G133" s="1">
         <v>6.3755559999999996</v>
@@ -8093,13 +8089,13 @@
         <v>6</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>472</v>
+        <v>261</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>288</v>
+        <v>463</v>
       </c>
       <c r="G134" s="1">
         <v>6.2</v>
@@ -8135,10 +8131,10 @@
         <v>107</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>289</v>
+        <v>464</v>
       </c>
       <c r="G135" s="1">
         <v>10.687778</v>
@@ -8171,13 +8167,13 @@
         <v>6</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>473</v>
+        <v>262</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>290</v>
+        <v>465</v>
       </c>
       <c r="G136" s="1">
         <v>8.1366669999999992</v>
@@ -8210,13 +8206,13 @@
         <v>6</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>474</v>
+        <v>263</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>291</v>
+        <v>466</v>
       </c>
       <c r="G137" s="1">
         <v>8.9488889999999994</v>
@@ -8249,13 +8245,13 @@
         <v>6</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>475</v>
+        <v>264</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>292</v>
+        <v>467</v>
       </c>
       <c r="G138" s="1">
         <v>6.3344440000000004</v>
@@ -8288,13 +8284,13 @@
         <v>6</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>476</v>
+        <v>265</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>293</v>
+        <v>468</v>
       </c>
       <c r="G139" s="1">
         <v>7.6577780000000004</v>
@@ -8327,13 +8323,13 @@
         <v>6</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>477</v>
+        <v>266</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>294</v>
+        <v>469</v>
       </c>
       <c r="G140" s="1">
         <v>8.01</v>
@@ -8366,13 +8362,13 @@
         <v>6</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>478</v>
+        <v>267</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>295</v>
+        <v>470</v>
       </c>
       <c r="G141" s="1">
         <v>8.5111109999999996</v>
@@ -8408,10 +8404,10 @@
         <v>113</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>296</v>
+        <v>471</v>
       </c>
       <c r="G142" s="1">
         <v>9.4955560000000006</v>
@@ -8447,10 +8443,10 @@
         <v>115</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>297</v>
+        <v>472</v>
       </c>
       <c r="G143" s="1">
         <v>9.1677780000000002</v>
@@ -8483,13 +8479,13 @@
         <v>6</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>460</v>
+        <v>249</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>298</v>
+        <v>473</v>
       </c>
       <c r="G144" s="1">
         <v>7.7311110000000003</v>
@@ -8522,13 +8518,13 @@
         <v>6</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>479</v>
+        <v>268</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
       <c r="G145" s="1">
         <v>8.5744439999999997</v>
@@ -8561,13 +8557,13 @@
         <v>6</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>376</v>
+        <v>165</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>299</v>
+        <v>474</v>
       </c>
       <c r="G146" s="1">
         <v>7.1577780000000004</v>
@@ -8600,13 +8596,13 @@
         <v>6</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>480</v>
+        <v>269</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>300</v>
+        <v>475</v>
       </c>
       <c r="G147" s="1">
         <v>9.0733329999999999</v>
@@ -8639,13 +8635,13 @@
         <v>6</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>481</v>
+        <v>270</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>233</v>
+        <v>408</v>
       </c>
       <c r="G148" s="1">
         <v>8.0633330000000001</v>
@@ -8678,13 +8674,13 @@
         <v>6</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>482</v>
+        <v>271</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>301</v>
+        <v>476</v>
       </c>
       <c r="G149" s="1">
         <v>7.8133330000000001</v>
@@ -8717,13 +8713,13 @@
         <v>6</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>483</v>
+        <v>272</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>302</v>
+        <v>477</v>
       </c>
       <c r="G150" s="1">
         <v>9.4488889999999994</v>
@@ -8756,13 +8752,13 @@
         <v>6</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>484</v>
+        <v>273</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>303</v>
+        <v>478</v>
       </c>
       <c r="G151" s="1">
         <v>8.927778</v>
@@ -8795,13 +8791,13 @@
         <v>6</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>485</v>
+        <v>274</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>304</v>
+        <v>479</v>
       </c>
       <c r="G152" s="1">
         <v>5.782222</v>
@@ -8834,13 +8830,13 @@
         <v>6</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>486</v>
+        <v>275</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>305</v>
+        <v>480</v>
       </c>
       <c r="G153" s="1">
         <v>10.626666999999999</v>
@@ -8873,13 +8869,13 @@
         <v>6</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>487</v>
+        <v>276</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>306</v>
+        <v>481</v>
       </c>
       <c r="G154" s="1">
         <v>10.188889</v>
@@ -8915,10 +8911,10 @@
         <v>67</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>307</v>
+        <v>482</v>
       </c>
       <c r="G155" s="1">
         <v>10.313333</v>
@@ -8954,10 +8950,10 @@
         <v>94</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
       <c r="G156" s="1">
         <v>8.7511109999999999</v>
@@ -8990,13 +8986,13 @@
         <v>6</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>488</v>
+        <v>277</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>308</v>
+        <v>483</v>
       </c>
       <c r="G157" s="1">
         <v>7.96</v>
@@ -9029,13 +9025,13 @@
         <v>6</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>489</v>
+        <v>278</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
       <c r="G158" s="1">
         <v>8.73</v>
@@ -9068,13 +9064,13 @@
         <v>6</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>490</v>
+        <v>279</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>309</v>
+        <v>484</v>
       </c>
       <c r="G159" s="1">
         <v>8.3344439999999995</v>
@@ -9107,13 +9103,13 @@
         <v>6</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>491</v>
+        <v>280</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>310</v>
+        <v>485</v>
       </c>
       <c r="G160" s="1">
         <v>10.813333</v>
@@ -9146,13 +9142,13 @@
         <v>6</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>492</v>
+        <v>281</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>311</v>
+        <v>486</v>
       </c>
       <c r="G161" s="1">
         <v>11.303333</v>
@@ -9185,13 +9181,13 @@
         <v>6</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>493</v>
+        <v>282</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>233</v>
+        <v>408</v>
       </c>
       <c r="G162" s="1">
         <v>11.928889</v>
@@ -9224,13 +9220,13 @@
         <v>6</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>446</v>
+        <v>235</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>312</v>
+        <v>487</v>
       </c>
       <c r="G163" s="1">
         <v>12.553333</v>
@@ -9263,13 +9259,13 @@
         <v>6</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>494</v>
+        <v>283</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>313</v>
+        <v>488</v>
       </c>
       <c r="G164" s="1">
         <v>9.7177779999999991</v>
@@ -9305,10 +9301,10 @@
         <v>123</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>314</v>
+        <v>489</v>
       </c>
       <c r="G165" s="1">
         <v>7.3244439999999997</v>
@@ -9341,13 +9337,13 @@
         <v>6</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>495</v>
+        <v>284</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>315</v>
+        <v>490</v>
       </c>
       <c r="G166" s="1">
         <v>8.5111109999999996</v>
@@ -9380,13 +9376,13 @@
         <v>6</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>496</v>
+        <v>285</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>316</v>
+        <v>491</v>
       </c>
       <c r="G167" s="1">
         <v>7.104444</v>
@@ -9419,13 +9415,13 @@
         <v>6</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>488</v>
+        <v>277</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>317</v>
+        <v>492</v>
       </c>
       <c r="G168" s="1">
         <v>8.177778</v>
@@ -9458,13 +9454,13 @@
         <v>6</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>497</v>
+        <v>286</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>318</v>
+        <v>493</v>
       </c>
       <c r="G169" s="1">
         <v>7.72</v>
@@ -9497,13 +9493,13 @@
         <v>6</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>498</v>
+        <v>287</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>319</v>
+        <v>494</v>
       </c>
       <c r="G170" s="1">
         <v>6.8511110000000004</v>
@@ -9536,13 +9532,13 @@
         <v>6</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>499</v>
+        <v>288</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>320</v>
+        <v>495</v>
       </c>
       <c r="G171" s="1">
         <v>10.687778</v>
@@ -9575,13 +9571,13 @@
         <v>6</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>500</v>
+        <v>289</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>321</v>
+        <v>496</v>
       </c>
       <c r="G172" s="1">
         <v>9.177778</v>
@@ -9614,13 +9610,13 @@
         <v>6</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>501</v>
+        <v>290</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>322</v>
+        <v>497</v>
       </c>
       <c r="G173" s="1">
         <v>8.3866669999999992</v>
@@ -9653,13 +9649,13 @@
         <v>6</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>502</v>
+        <v>291</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>323</v>
+        <v>498</v>
       </c>
       <c r="G174" s="1">
         <v>5.855556</v>
@@ -9692,13 +9688,13 @@
         <v>6</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>503</v>
+        <v>292</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>324</v>
+        <v>499</v>
       </c>
       <c r="G175" s="1">
         <v>10.501111</v>
@@ -9731,13 +9727,13 @@
         <v>6</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>504</v>
+        <v>293</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>325</v>
+        <v>500</v>
       </c>
       <c r="G176" s="1">
         <v>8.1677780000000002</v>
@@ -9770,13 +9766,13 @@
         <v>6</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>505</v>
+        <v>294</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>326</v>
+        <v>501</v>
       </c>
       <c r="G177" s="1">
         <v>7.354444</v>
@@ -9812,10 +9808,10 @@
         <v>133</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>327</v>
+        <v>502</v>
       </c>
       <c r="G178" s="1">
         <v>7.8033330000000003</v>
@@ -9848,13 +9844,13 @@
         <v>6</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>506</v>
+        <v>295</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="G179" s="1">
         <v>8.1999999999999993</v>
@@ -9887,13 +9883,13 @@
         <v>6</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>507</v>
+        <v>296</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>329</v>
+        <v>504</v>
       </c>
       <c r="G180" s="1">
         <v>8.4288889999999999</v>
@@ -9926,13 +9922,13 @@
         <v>6</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>508</v>
+        <v>297</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>330</v>
+        <v>505</v>
       </c>
       <c r="G181" s="1">
         <v>9.855556</v>
@@ -9965,13 +9961,13 @@
         <v>6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>509</v>
+        <v>298</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>331</v>
+        <v>506</v>
       </c>
       <c r="G182" s="1">
         <v>8.8866669999999992</v>
@@ -10004,13 +10000,13 @@
         <v>6</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>510</v>
+        <v>299</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>332</v>
+        <v>507</v>
       </c>
       <c r="G183" s="1">
         <v>7.9377779999999998</v>
@@ -10043,13 +10039,13 @@
         <v>6</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>511</v>
+        <v>300</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>333</v>
+        <v>508</v>
       </c>
       <c r="G184" s="1">
         <v>8.3244439999999997</v>
@@ -10085,10 +10081,10 @@
         <v>135</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>334</v>
+        <v>509</v>
       </c>
       <c r="G185" s="1">
         <v>10.365556</v>
@@ -10121,13 +10117,13 @@
         <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>512</v>
+        <v>301</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>335</v>
+        <v>510</v>
       </c>
       <c r="G186" s="1">
         <v>9.8133330000000001</v>
@@ -10160,13 +10156,13 @@
         <v>6</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>513</v>
+        <v>302</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>336</v>
+        <v>511</v>
       </c>
       <c r="G187" s="1">
         <v>10.72</v>
@@ -10199,13 +10195,13 @@
         <v>6</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>514</v>
+        <v>303</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>337</v>
+        <v>512</v>
       </c>
       <c r="G188" s="1">
         <v>7.72</v>
@@ -10238,13 +10234,13 @@
         <v>6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>515</v>
+        <v>304</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>338</v>
+        <v>513</v>
       </c>
       <c r="G189" s="1">
         <v>8.5122219999999995</v>
@@ -10277,13 +10273,13 @@
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>516</v>
+        <v>305</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>339</v>
+        <v>514</v>
       </c>
       <c r="G190" s="1">
         <v>7.0111109999999996</v>
@@ -10316,13 +10312,13 @@
         <v>6</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>517</v>
+        <v>306</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>340</v>
+        <v>515</v>
       </c>
       <c r="G191" s="1">
         <v>8.7200000000000006</v>
@@ -10355,13 +10351,13 @@
         <v>6</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>518</v>
+        <v>307</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>341</v>
+        <v>516</v>
       </c>
       <c r="G192" s="1">
         <v>10.48</v>
@@ -10394,13 +10390,13 @@
         <v>6</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>519</v>
+        <v>308</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>192</v>
+        <v>367</v>
       </c>
       <c r="G193" s="1">
         <v>11.698888999999999</v>
@@ -10436,10 +10432,10 @@
         <v>137</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>342</v>
+        <v>517</v>
       </c>
       <c r="G194" s="1">
         <v>7.3855560000000002</v>
@@ -10472,13 +10468,13 @@
         <v>6</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>520</v>
+        <v>309</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>343</v>
+        <v>518</v>
       </c>
       <c r="G195" s="1">
         <v>8.0222219999999993</v>
@@ -10511,13 +10507,13 @@
         <v>6</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>521</v>
+        <v>310</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>344</v>
+        <v>519</v>
       </c>
       <c r="G196" s="1">
         <v>9.855556</v>
@@ -10550,13 +10546,13 @@
         <v>6</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>522</v>
+        <v>311</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>345</v>
+        <v>520</v>
       </c>
       <c r="G197" s="1">
         <v>6.7088890000000001</v>
@@ -10589,13 +10585,13 @@
         <v>6</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>523</v>
+        <v>312</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>346</v>
+        <v>521</v>
       </c>
       <c r="G198" s="1">
         <v>8.4911110000000001</v>
@@ -10631,10 +10627,10 @@
         <v>138</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>347</v>
+        <v>522</v>
       </c>
       <c r="G199" s="1">
         <v>9.0522220000000004</v>
@@ -10667,13 +10663,13 @@
         <v>6</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>524</v>
+        <v>313</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>348</v>
+        <v>523</v>
       </c>
       <c r="G200" s="1">
         <v>9.7088889999999992</v>
@@ -10706,13 +10702,13 @@
         <v>6</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>525</v>
+        <v>314</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>349</v>
+        <v>524</v>
       </c>
       <c r="G201" s="1">
         <v>9.8033330000000003</v>
@@ -10745,13 +10741,13 @@
         <v>6</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>526</v>
+        <v>315</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>350</v>
+        <v>525</v>
       </c>
       <c r="G202" s="1">
         <v>9.2722219999999993</v>
@@ -10784,13 +10780,13 @@
         <v>6</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>527</v>
+        <v>316</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>351</v>
+        <v>526</v>
       </c>
       <c r="G203" s="1">
         <v>8.9488889999999994</v>
@@ -10823,13 +10819,13 @@
         <v>6</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>528</v>
+        <v>317</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>352</v>
+        <v>527</v>
       </c>
       <c r="G204" s="1">
         <v>8.1677780000000002</v>
@@ -10862,13 +10858,13 @@
         <v>6</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>529</v>
+        <v>318</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>353</v>
+        <v>528</v>
       </c>
       <c r="G205" s="1">
         <v>7.73</v>
@@ -10901,13 +10897,13 @@
         <v>6</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>530</v>
+        <v>319</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>354</v>
+        <v>529</v>
       </c>
       <c r="G206" s="1">
         <v>10.032222000000001</v>
@@ -10943,10 +10939,10 @@
         <v>139</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>355</v>
+        <v>530</v>
       </c>
       <c r="G207" s="1">
         <v>7.9488890000000003</v>
@@ -10982,10 +10978,10 @@
         <v>141</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>356</v>
+        <v>531</v>
       </c>
       <c r="G208" s="1">
         <v>7.5944440000000002</v>
@@ -11018,13 +11014,13 @@
         <v>6</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>531</v>
+        <v>320</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>357</v>
+        <v>532</v>
       </c>
       <c r="G209" s="1">
         <v>9.1577780000000004</v>
@@ -11057,13 +11053,13 @@
         <v>6</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>532</v>
+        <v>321</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>358</v>
+        <v>533</v>
       </c>
       <c r="G210" s="1">
         <v>9.8033330000000003</v>
@@ -11096,13 +11092,13 @@
         <v>6</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>533</v>
+        <v>322</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>359</v>
+        <v>534</v>
       </c>
       <c r="G211" s="1">
         <v>7.6155559999999998</v>
@@ -11135,13 +11131,13 @@
         <v>6</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>534</v>
+        <v>323</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>360</v>
+        <v>535</v>
       </c>
       <c r="G212" s="1">
         <v>10.272221999999999</v>
@@ -11174,13 +11170,13 @@
         <v>6</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>535</v>
+        <v>324</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>361</v>
+        <v>536</v>
       </c>
       <c r="G213" s="1">
         <v>8.6044440000000009</v>
@@ -11213,13 +11209,13 @@
         <v>6</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>536</v>
+        <v>325</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>362</v>
+        <v>537</v>
       </c>
       <c r="G214" s="1">
         <v>9.0011109999999999</v>
@@ -11252,13 +11248,13 @@
         <v>6</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>537</v>
+        <v>326</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>363</v>
+        <v>538</v>
       </c>
       <c r="G215" s="1">
         <v>6.5433329999999996</v>
@@ -11291,13 +11287,13 @@
         <v>6</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>538</v>
+        <v>327</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>364</v>
+        <v>539</v>
       </c>
       <c r="G216" s="1">
         <v>8.4388889999999996</v>
@@ -11330,13 +11326,13 @@
         <v>6</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>539</v>
+        <v>328</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>365</v>
+        <v>540</v>
       </c>
       <c r="G217" s="1">
         <v>5.9177780000000002</v>
@@ -11369,13 +11365,13 @@
         <v>6</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>540</v>
+        <v>329</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
       <c r="G218" s="1">
         <v>10.741111</v>
@@ -11408,13 +11404,13 @@
         <v>6</v>
       </c>
       <c r="D219" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F219" s="1" t="s">
         <v>541</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="G219" s="1">
         <v>8.5944439999999993</v>
@@ -11447,13 +11443,13 @@
         <v>6</v>
       </c>
       <c r="D220" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F220" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="G220" s="1">
         <v>7.605556</v>
@@ -11486,13 +11482,13 @@
         <v>6</v>
       </c>
       <c r="D221" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F221" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F221" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="G221" s="1">
         <v>8.2355560000000008</v>

</xml_diff>

<commit_message>
sleep sleep prediction update
</commit_message>
<xml_diff>
--- a/SlpGroupInfo.xlsx
+++ b/SlpGroupInfo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="545">
   <si>
     <t>SubjId</t>
   </si>
@@ -1652,6 +1652,9 @@
   </si>
   <si>
     <t>[0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0]</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
@@ -1858,11 +1861,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2120493064"/>
-        <c:axId val="-2120639784"/>
+        <c:axId val="2120770328"/>
+        <c:axId val="2120779320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2120493064"/>
+        <c:axId val="2120770328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +1908,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120639784"/>
+        <c:crossAx val="2120779320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1913,7 +1916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120639784"/>
+        <c:axId val="2120779320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1964,7 +1967,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120493064"/>
+        <c:crossAx val="2120770328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2878,10 +2881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L221"/>
+  <dimension ref="A1:M221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="G217" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2892,7 +2895,7 @@
     <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2929,8 +2932,11 @@
       <c r="L1" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2968,8 +2974,11 @@
       <c r="L2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -3007,8 +3016,11 @@
       <c r="L3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3046,8 +3058,11 @@
       <c r="L4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3085,8 +3100,11 @@
       <c r="L5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3124,8 +3142,11 @@
       <c r="L6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3163,8 +3184,11 @@
       <c r="L7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3202,8 +3226,11 @@
       <c r="L8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3241,8 +3268,11 @@
       <c r="L9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -3280,8 +3310,11 @@
       <c r="L10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -3319,8 +3352,11 @@
       <c r="L11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -3358,8 +3394,11 @@
       <c r="L12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -3397,8 +3436,11 @@
       <c r="L13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -3436,8 +3478,11 @@
       <c r="L14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -3475,8 +3520,11 @@
       <c r="L15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -3514,8 +3562,11 @@
       <c r="L16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -3553,8 +3604,11 @@
       <c r="L17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -3592,8 +3646,11 @@
       <c r="L18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -3631,8 +3688,11 @@
       <c r="L19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -3670,8 +3730,11 @@
       <c r="L20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -3709,8 +3772,11 @@
       <c r="L21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -3748,8 +3814,11 @@
       <c r="L22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -3787,8 +3856,11 @@
       <c r="L23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -3826,8 +3898,11 @@
       <c r="L24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -3865,8 +3940,11 @@
       <c r="L25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -3904,8 +3982,11 @@
       <c r="L26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -3943,8 +4024,11 @@
       <c r="L27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -3982,8 +4066,11 @@
       <c r="L28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -4021,8 +4108,11 @@
       <c r="L29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -4060,8 +4150,11 @@
       <c r="L30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -4099,8 +4192,11 @@
       <c r="L31" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -4138,8 +4234,11 @@
       <c r="L32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -4177,8 +4276,11 @@
       <c r="L33" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -4216,8 +4318,11 @@
       <c r="L34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -4255,8 +4360,11 @@
       <c r="L35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -4294,8 +4402,11 @@
       <c r="L36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -4333,8 +4444,11 @@
       <c r="L37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -4372,8 +4486,11 @@
       <c r="L38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -4411,8 +4528,11 @@
       <c r="L39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -4450,8 +4570,11 @@
       <c r="L40" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -4489,8 +4612,11 @@
       <c r="L41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -4528,8 +4654,11 @@
       <c r="L42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -4567,8 +4696,11 @@
       <c r="L43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -4606,8 +4738,11 @@
       <c r="L44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -4645,8 +4780,11 @@
       <c r="L45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
@@ -4684,8 +4822,11 @@
       <c r="L46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -4723,8 +4864,11 @@
       <c r="L47" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
@@ -4762,8 +4906,11 @@
       <c r="L48" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -4801,8 +4948,11 @@
       <c r="L49" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
@@ -4840,8 +4990,11 @@
       <c r="L50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -4879,8 +5032,11 @@
       <c r="L51" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -4918,8 +5074,11 @@
       <c r="L52" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="M52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -4957,8 +5116,11 @@
       <c r="L53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -4996,8 +5158,11 @@
       <c r="L54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -5035,8 +5200,11 @@
       <c r="L55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -5074,8 +5242,11 @@
       <c r="L56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
@@ -5113,8 +5284,11 @@
       <c r="L57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -5152,8 +5326,11 @@
       <c r="L58" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -5191,8 +5368,11 @@
       <c r="L59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -5230,8 +5410,11 @@
       <c r="L60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
@@ -5269,8 +5452,11 @@
       <c r="L61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -5308,8 +5494,11 @@
       <c r="L62" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -5347,8 +5536,11 @@
       <c r="L63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="M63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -5386,8 +5578,11 @@
       <c r="L64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="M64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -5425,8 +5620,11 @@
       <c r="L65" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="M65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -5464,8 +5662,11 @@
       <c r="L66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="M66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
@@ -5503,8 +5704,11 @@
       <c r="L67" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="M67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -5542,8 +5746,11 @@
       <c r="L68" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="M68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -5581,8 +5788,11 @@
       <c r="L69" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="1" t="s">
         <v>65</v>
       </c>
@@ -5620,8 +5830,11 @@
       <c r="L70" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" s="1" t="s">
         <v>65</v>
       </c>
@@ -5659,8 +5872,11 @@
       <c r="L71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="M71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -5698,8 +5914,11 @@
       <c r="L72" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="M72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -5737,8 +5956,11 @@
       <c r="L73" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="M73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -5776,8 +5998,11 @@
       <c r="L74" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="M74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -5815,8 +6040,11 @@
       <c r="L75" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="M75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
       <c r="A76" s="1" t="s">
         <v>78</v>
       </c>
@@ -5854,8 +6082,11 @@
       <c r="L76" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="M76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
@@ -5893,8 +6124,11 @@
       <c r="L77" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="M77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
@@ -5932,8 +6166,11 @@
       <c r="L78" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="M78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -5971,8 +6208,11 @@
       <c r="L79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="M79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -6010,8 +6250,11 @@
       <c r="L80" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="M80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -6049,8 +6292,11 @@
       <c r="L81" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="M81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" s="1" t="s">
         <v>78</v>
       </c>
@@ -6088,8 +6334,11 @@
       <c r="L82" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="M82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
       <c r="A83" s="1" t="s">
         <v>78</v>
       </c>
@@ -6127,8 +6376,11 @@
       <c r="L83" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="M83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" s="1" t="s">
         <v>78</v>
       </c>
@@ -6166,8 +6418,11 @@
       <c r="L84" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="M84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" s="1" t="s">
         <v>78</v>
       </c>
@@ -6205,8 +6460,11 @@
       <c r="L85" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="M85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -6244,8 +6502,11 @@
       <c r="L86" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="M86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -6283,8 +6544,11 @@
       <c r="L87" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="M87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -6322,8 +6586,11 @@
       <c r="L88" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="M88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -6361,8 +6628,11 @@
       <c r="L89" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="M89" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -6400,8 +6670,11 @@
       <c r="L90" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="M90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" s="1" t="s">
         <v>85</v>
       </c>
@@ -6439,8 +6712,11 @@
       <c r="L91" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:12">
+      <c r="M91" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" s="1" t="s">
         <v>85</v>
       </c>
@@ -6478,8 +6754,11 @@
       <c r="L92" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:12">
+      <c r="M92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" s="1" t="s">
         <v>85</v>
       </c>
@@ -6517,8 +6796,11 @@
       <c r="L93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:12">
+      <c r="M93" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" s="1" t="s">
         <v>85</v>
       </c>
@@ -6556,8 +6838,11 @@
       <c r="L94" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="M94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" s="1" t="s">
         <v>85</v>
       </c>
@@ -6595,8 +6880,11 @@
       <c r="L95" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:12">
+      <c r="M95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" s="1" t="s">
         <v>85</v>
       </c>
@@ -6634,8 +6922,11 @@
       <c r="L96" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:12">
+      <c r="M96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
       <c r="A97" s="1" t="s">
         <v>90</v>
       </c>
@@ -6673,8 +6964,11 @@
       <c r="L97" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:12">
+      <c r="M97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" s="1" t="s">
         <v>90</v>
       </c>
@@ -6712,8 +7006,11 @@
       <c r="L98" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:12">
+      <c r="M98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" s="1" t="s">
         <v>90</v>
       </c>
@@ -6751,8 +7048,11 @@
       <c r="L99" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:12">
+      <c r="M99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
         <v>90</v>
       </c>
@@ -6790,8 +7090,11 @@
       <c r="L100" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:12">
+      <c r="M100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
         <v>90</v>
       </c>
@@ -6829,8 +7132,11 @@
       <c r="L101" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:12">
+      <c r="M101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
         <v>90</v>
       </c>
@@ -6868,8 +7174,11 @@
       <c r="L102" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:12">
+      <c r="M102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
         <v>90</v>
       </c>
@@ -6907,8 +7216,11 @@
       <c r="L103" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:12">
+      <c r="M103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
         <v>90</v>
       </c>
@@ -6946,8 +7258,11 @@
       <c r="L104" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:12">
+      <c r="M104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
         <v>90</v>
       </c>
@@ -6985,8 +7300,11 @@
       <c r="L105" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:12">
+      <c r="M105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
         <v>90</v>
       </c>
@@ -7024,8 +7342,11 @@
       <c r="L106" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:12">
+      <c r="M106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
         <v>90</v>
       </c>
@@ -7063,8 +7384,11 @@
       <c r="L107" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:12">
+      <c r="M107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
         <v>90</v>
       </c>
@@ -7102,8 +7426,11 @@
       <c r="L108" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:12">
+      <c r="M108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
         <v>90</v>
       </c>
@@ -7141,8 +7468,11 @@
       <c r="L109" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:12">
+      <c r="M109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
         <v>90</v>
       </c>
@@ -7180,8 +7510,11 @@
       <c r="L110" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:12">
+      <c r="M110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
         <v>93</v>
       </c>
@@ -7219,8 +7552,11 @@
       <c r="L111" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:12">
+      <c r="M111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
         <v>93</v>
       </c>
@@ -7258,8 +7594,11 @@
       <c r="L112" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:12">
+      <c r="M112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13">
       <c r="A113" s="1" t="s">
         <v>93</v>
       </c>
@@ -7297,8 +7636,11 @@
       <c r="L113" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:12">
+      <c r="M113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13">
       <c r="A114" s="1" t="s">
         <v>93</v>
       </c>
@@ -7336,8 +7678,11 @@
       <c r="L114" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:12">
+      <c r="M114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13">
       <c r="A115" s="1" t="s">
         <v>93</v>
       </c>
@@ -7375,8 +7720,11 @@
       <c r="L115" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:12">
+      <c r="M115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13">
       <c r="A116" s="1" t="s">
         <v>93</v>
       </c>
@@ -7414,8 +7762,11 @@
       <c r="L116" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:12">
+      <c r="M116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13">
       <c r="A117" s="1" t="s">
         <v>93</v>
       </c>
@@ -7453,8 +7804,11 @@
       <c r="L117" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:12">
+      <c r="M117" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13">
       <c r="A118" s="1" t="s">
         <v>93</v>
       </c>
@@ -7492,8 +7846,11 @@
       <c r="L118" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:12">
+      <c r="M118" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
       <c r="A119" s="1" t="s">
         <v>93</v>
       </c>
@@ -7531,8 +7888,11 @@
       <c r="L119" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:12">
+      <c r="M119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13">
       <c r="A120" s="1" t="s">
         <v>93</v>
       </c>
@@ -7570,8 +7930,11 @@
       <c r="L120" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:12">
+      <c r="M120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13">
       <c r="A121" s="1" t="s">
         <v>93</v>
       </c>
@@ -7609,8 +7972,11 @@
       <c r="L121" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:12">
+      <c r="M121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13">
       <c r="A122" s="1" t="s">
         <v>93</v>
       </c>
@@ -7648,8 +8014,11 @@
       <c r="L122" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:12">
+      <c r="M122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13">
       <c r="A123" s="1" t="s">
         <v>93</v>
       </c>
@@ -7687,8 +8056,11 @@
       <c r="L123" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:12">
+      <c r="M123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13">
       <c r="A124" s="1" t="s">
         <v>97</v>
       </c>
@@ -7726,8 +8098,11 @@
       <c r="L124" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:12">
+      <c r="M124" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
       <c r="A125" s="1" t="s">
         <v>97</v>
       </c>
@@ -7765,8 +8140,11 @@
       <c r="L125" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:12">
+      <c r="M125" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
       <c r="A126" s="1" t="s">
         <v>97</v>
       </c>
@@ -7804,8 +8182,11 @@
       <c r="L126" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:12">
+      <c r="M126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
       <c r="A127" s="1" t="s">
         <v>97</v>
       </c>
@@ -7843,8 +8224,11 @@
       <c r="L127" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:12">
+      <c r="M127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
       <c r="A128" s="1" t="s">
         <v>97</v>
       </c>
@@ -7882,8 +8266,11 @@
       <c r="L128" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:12">
+      <c r="M128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13">
       <c r="A129" s="1" t="s">
         <v>97</v>
       </c>
@@ -7921,8 +8308,11 @@
       <c r="L129" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:12">
+      <c r="M129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13">
       <c r="A130" s="1" t="s">
         <v>97</v>
       </c>
@@ -7960,8 +8350,11 @@
       <c r="L130" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:12">
+      <c r="M130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
       <c r="A131" s="1" t="s">
         <v>97</v>
       </c>
@@ -7999,8 +8392,11 @@
       <c r="L131" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:12">
+      <c r="M131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13">
       <c r="A132" s="1" t="s">
         <v>97</v>
       </c>
@@ -8038,8 +8434,11 @@
       <c r="L132" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:12">
+      <c r="M132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
       <c r="A133" s="1" t="s">
         <v>102</v>
       </c>
@@ -8077,8 +8476,11 @@
       <c r="L133" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:12">
+      <c r="M133" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13">
       <c r="A134" s="1" t="s">
         <v>102</v>
       </c>
@@ -8116,8 +8518,11 @@
       <c r="L134" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:12">
+      <c r="M134" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13">
       <c r="A135" s="1" t="s">
         <v>102</v>
       </c>
@@ -8155,8 +8560,11 @@
       <c r="L135" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:12">
+      <c r="M135" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13">
       <c r="A136" s="1" t="s">
         <v>102</v>
       </c>
@@ -8194,8 +8602,11 @@
       <c r="L136" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:12">
+      <c r="M136" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13">
       <c r="A137" s="1" t="s">
         <v>102</v>
       </c>
@@ -8233,8 +8644,11 @@
       <c r="L137" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:12">
+      <c r="M137" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13">
       <c r="A138" s="1" t="s">
         <v>102</v>
       </c>
@@ -8272,8 +8686,11 @@
       <c r="L138" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:12">
+      <c r="M138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13">
       <c r="A139" s="1" t="s">
         <v>102</v>
       </c>
@@ -8311,8 +8728,11 @@
       <c r="L139" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:12">
+      <c r="M139" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13">
       <c r="A140" s="1" t="s">
         <v>112</v>
       </c>
@@ -8350,8 +8770,11 @@
       <c r="L140" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:12">
+      <c r="M140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13">
       <c r="A141" s="1" t="s">
         <v>112</v>
       </c>
@@ -8389,8 +8812,11 @@
       <c r="L141" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:12">
+      <c r="M141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13">
       <c r="A142" s="1" t="s">
         <v>112</v>
       </c>
@@ -8428,8 +8854,11 @@
       <c r="L142" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:12">
+      <c r="M142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13">
       <c r="A143" s="1" t="s">
         <v>114</v>
       </c>
@@ -8467,8 +8896,11 @@
       <c r="L143" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:12">
+      <c r="M143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13">
       <c r="A144" s="1" t="s">
         <v>114</v>
       </c>
@@ -8506,8 +8938,11 @@
       <c r="L144" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:12">
+      <c r="M144" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13">
       <c r="A145" s="1" t="s">
         <v>114</v>
       </c>
@@ -8545,8 +8980,11 @@
       <c r="L145" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:12">
+      <c r="M145" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13">
       <c r="A146" s="1" t="s">
         <v>114</v>
       </c>
@@ -8584,8 +9022,11 @@
       <c r="L146" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:12">
+      <c r="M146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13">
       <c r="A147" s="1" t="s">
         <v>114</v>
       </c>
@@ -8623,8 +9064,11 @@
       <c r="L147" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:12">
+      <c r="M147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13">
       <c r="A148" s="1" t="s">
         <v>114</v>
       </c>
@@ -8662,8 +9106,11 @@
       <c r="L148" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:12">
+      <c r="M148" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13">
       <c r="A149" s="1" t="s">
         <v>114</v>
       </c>
@@ -8701,8 +9148,11 @@
       <c r="L149" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:12">
+      <c r="M149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13">
       <c r="A150" s="1" t="s">
         <v>114</v>
       </c>
@@ -8740,8 +9190,11 @@
       <c r="L150" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:12">
+      <c r="M150" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13">
       <c r="A151" s="1" t="s">
         <v>114</v>
       </c>
@@ -8779,8 +9232,11 @@
       <c r="L151" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:12">
+      <c r="M151" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13">
       <c r="A152" s="1" t="s">
         <v>114</v>
       </c>
@@ -8818,8 +9274,11 @@
       <c r="L152" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:12">
+      <c r="M152" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13">
       <c r="A153" s="1" t="s">
         <v>114</v>
       </c>
@@ -8857,8 +9316,11 @@
       <c r="L153" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:12">
+      <c r="M153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13">
       <c r="A154" s="1" t="s">
         <v>114</v>
       </c>
@@ -8896,8 +9358,11 @@
       <c r="L154" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:12">
+      <c r="M154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13">
       <c r="A155" s="1" t="s">
         <v>114</v>
       </c>
@@ -8935,8 +9400,11 @@
       <c r="L155" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:12">
+      <c r="M155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13">
       <c r="A156" s="1" t="s">
         <v>120</v>
       </c>
@@ -8974,8 +9442,11 @@
       <c r="L156" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:12">
+      <c r="M156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13">
       <c r="A157" s="1" t="s">
         <v>120</v>
       </c>
@@ -9013,8 +9484,11 @@
       <c r="L157" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:12">
+      <c r="M157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13">
       <c r="A158" s="1" t="s">
         <v>120</v>
       </c>
@@ -9052,8 +9526,11 @@
       <c r="L158" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:12">
+      <c r="M158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13">
       <c r="A159" s="1" t="s">
         <v>120</v>
       </c>
@@ -9091,8 +9568,11 @@
       <c r="L159" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:12">
+      <c r="M159" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13">
       <c r="A160" s="1" t="s">
         <v>120</v>
       </c>
@@ -9130,8 +9610,11 @@
       <c r="L160" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:12">
+      <c r="M160" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13">
       <c r="A161" s="1" t="s">
         <v>120</v>
       </c>
@@ -9169,8 +9652,11 @@
       <c r="L161" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:12">
+      <c r="M161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13">
       <c r="A162" s="1" t="s">
         <v>120</v>
       </c>
@@ -9208,8 +9694,11 @@
       <c r="L162" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:12">
+      <c r="M162" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13">
       <c r="A163" s="1" t="s">
         <v>120</v>
       </c>
@@ -9247,8 +9736,11 @@
       <c r="L163" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:12">
+      <c r="M163" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13">
       <c r="A164" s="1" t="s">
         <v>120</v>
       </c>
@@ -9286,8 +9778,11 @@
       <c r="L164" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:12">
+      <c r="M164" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13">
       <c r="A165" s="1" t="s">
         <v>122</v>
       </c>
@@ -9325,8 +9820,11 @@
       <c r="L165" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:12">
+      <c r="M165" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13">
       <c r="A166" s="1" t="s">
         <v>122</v>
       </c>
@@ -9364,8 +9862,11 @@
       <c r="L166" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:12">
+      <c r="M166" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13">
       <c r="A167" s="1" t="s">
         <v>122</v>
       </c>
@@ -9403,8 +9904,11 @@
       <c r="L167" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:12">
+      <c r="M167" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13">
       <c r="A168" s="1" t="s">
         <v>122</v>
       </c>
@@ -9442,8 +9946,11 @@
       <c r="L168" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:12">
+      <c r="M168" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13">
       <c r="A169" s="1" t="s">
         <v>122</v>
       </c>
@@ -9481,8 +9988,11 @@
       <c r="L169" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:12">
+      <c r="M169" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13">
       <c r="A170" s="1" t="s">
         <v>122</v>
       </c>
@@ -9520,8 +10030,11 @@
       <c r="L170" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:12">
+      <c r="M170" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13">
       <c r="A171" s="1" t="s">
         <v>124</v>
       </c>
@@ -9559,8 +10072,11 @@
       <c r="L171" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:12">
+      <c r="M171" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13">
       <c r="A172" s="1" t="s">
         <v>124</v>
       </c>
@@ -9598,8 +10114,11 @@
       <c r="L172" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:12">
+      <c r="M172" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13">
       <c r="A173" s="1" t="s">
         <v>124</v>
       </c>
@@ -9637,8 +10156,11 @@
       <c r="L173" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:12">
+      <c r="M173" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13">
       <c r="A174" s="1" t="s">
         <v>124</v>
       </c>
@@ -9676,8 +10198,11 @@
       <c r="L174" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:12">
+      <c r="M174" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13">
       <c r="A175" s="1" t="s">
         <v>124</v>
       </c>
@@ -9715,8 +10240,11 @@
       <c r="L175" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:12">
+      <c r="M175" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13">
       <c r="A176" s="1" t="s">
         <v>124</v>
       </c>
@@ -9754,8 +10282,11 @@
       <c r="L176" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:12">
+      <c r="M176" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13">
       <c r="A177" s="1" t="s">
         <v>124</v>
       </c>
@@ -9793,8 +10324,11 @@
       <c r="L177" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:12">
+      <c r="M177" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13">
       <c r="A178" s="1" t="s">
         <v>132</v>
       </c>
@@ -9832,8 +10366,11 @@
       <c r="L178" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:12">
+      <c r="M178" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13">
       <c r="A179" s="1" t="s">
         <v>132</v>
       </c>
@@ -9871,8 +10408,11 @@
       <c r="L179" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:12">
+      <c r="M179" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13">
       <c r="A180" s="1" t="s">
         <v>132</v>
       </c>
@@ -9910,8 +10450,11 @@
       <c r="L180" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:12">
+      <c r="M180" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13">
       <c r="A181" s="1" t="s">
         <v>132</v>
       </c>
@@ -9949,8 +10492,11 @@
       <c r="L181" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:12">
+      <c r="M181" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13">
       <c r="A182" s="1" t="s">
         <v>132</v>
       </c>
@@ -9988,8 +10534,11 @@
       <c r="L182" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:12">
+      <c r="M182" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13">
       <c r="A183" s="1" t="s">
         <v>132</v>
       </c>
@@ -10027,8 +10576,11 @@
       <c r="L183" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:12">
+      <c r="M183" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13">
       <c r="A184" s="1" t="s">
         <v>132</v>
       </c>
@@ -10066,8 +10618,11 @@
       <c r="L184" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:12">
+      <c r="M184" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13">
       <c r="A185" s="1" t="s">
         <v>134</v>
       </c>
@@ -10105,8 +10660,11 @@
       <c r="L185" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:12">
+      <c r="M185" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13">
       <c r="A186" s="1" t="s">
         <v>134</v>
       </c>
@@ -10144,8 +10702,11 @@
       <c r="L186" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:12">
+      <c r="M186" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13">
       <c r="A187" s="1" t="s">
         <v>134</v>
       </c>
@@ -10183,8 +10744,11 @@
       <c r="L187" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:12">
+      <c r="M187" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13">
       <c r="A188" s="1" t="s">
         <v>134</v>
       </c>
@@ -10222,8 +10786,11 @@
       <c r="L188" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:12">
+      <c r="M188" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13">
       <c r="A189" s="1" t="s">
         <v>134</v>
       </c>
@@ -10261,8 +10828,11 @@
       <c r="L189" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:12">
+      <c r="M189" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13">
       <c r="A190" s="1" t="s">
         <v>134</v>
       </c>
@@ -10300,8 +10870,11 @@
       <c r="L190" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:12">
+      <c r="M190" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13">
       <c r="A191" s="1" t="s">
         <v>134</v>
       </c>
@@ -10339,8 +10912,11 @@
       <c r="L191" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:12">
+      <c r="M191" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13">
       <c r="A192" s="1" t="s">
         <v>134</v>
       </c>
@@ -10378,8 +10954,11 @@
       <c r="L192" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:12">
+      <c r="M192" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13">
       <c r="A193" s="1" t="s">
         <v>134</v>
       </c>
@@ -10417,8 +10996,11 @@
       <c r="L193" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:12">
+      <c r="M193" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13">
       <c r="A194" s="1" t="s">
         <v>136</v>
       </c>
@@ -10456,8 +11038,11 @@
       <c r="L194" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:12">
+      <c r="M194" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13">
       <c r="A195" s="1" t="s">
         <v>136</v>
       </c>
@@ -10495,8 +11080,11 @@
       <c r="L195" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:12">
+      <c r="M195" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13">
       <c r="A196" s="1" t="s">
         <v>136</v>
       </c>
@@ -10534,8 +11122,11 @@
       <c r="L196" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:12">
+      <c r="M196" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13">
       <c r="A197" s="1" t="s">
         <v>136</v>
       </c>
@@ -10573,8 +11164,11 @@
       <c r="L197" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:12">
+      <c r="M197" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
         <v>136</v>
       </c>
@@ -10612,8 +11206,11 @@
       <c r="L198" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:12">
+      <c r="M198" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
         <v>136</v>
       </c>
@@ -10651,8 +11248,11 @@
       <c r="L199" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:12">
+      <c r="M199" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
         <v>136</v>
       </c>
@@ -10690,8 +11290,11 @@
       <c r="L200" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:12">
+      <c r="M200" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
         <v>136</v>
       </c>
@@ -10729,8 +11332,11 @@
       <c r="L201" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:12">
+      <c r="M201" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
         <v>136</v>
       </c>
@@ -10768,8 +11374,11 @@
       <c r="L202" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:12">
+      <c r="M202" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
         <v>136</v>
       </c>
@@ -10807,8 +11416,11 @@
       <c r="L203" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:12">
+      <c r="M203" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
         <v>136</v>
       </c>
@@ -10846,8 +11458,11 @@
       <c r="L204" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:12">
+      <c r="M204" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
         <v>136</v>
       </c>
@@ -10885,8 +11500,11 @@
       <c r="L205" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:12">
+      <c r="M205" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
         <v>136</v>
       </c>
@@ -10924,8 +11542,11 @@
       <c r="L206" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:12">
+      <c r="M206" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
         <v>136</v>
       </c>
@@ -10963,8 +11584,11 @@
       <c r="L207" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:12">
+      <c r="M207" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
         <v>140</v>
       </c>
@@ -11002,8 +11626,11 @@
       <c r="L208" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:12">
+      <c r="M208" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13">
       <c r="A209" s="1" t="s">
         <v>140</v>
       </c>
@@ -11041,8 +11668,11 @@
       <c r="L209" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:12">
+      <c r="M209" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13">
       <c r="A210" s="1" t="s">
         <v>140</v>
       </c>
@@ -11080,8 +11710,11 @@
       <c r="L210" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:12">
+      <c r="M210" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13">
       <c r="A211" s="1" t="s">
         <v>140</v>
       </c>
@@ -11119,8 +11752,11 @@
       <c r="L211" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:12">
+      <c r="M211" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13">
       <c r="A212" s="1" t="s">
         <v>140</v>
       </c>
@@ -11158,8 +11794,11 @@
       <c r="L212" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:12">
+      <c r="M212" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13">
       <c r="A213" s="1" t="s">
         <v>140</v>
       </c>
@@ -11197,8 +11836,11 @@
       <c r="L213" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:12">
+      <c r="M213" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13">
       <c r="A214" s="1" t="s">
         <v>140</v>
       </c>
@@ -11236,8 +11878,11 @@
       <c r="L214" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:12">
+      <c r="M214" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13">
       <c r="A215" s="1" t="s">
         <v>140</v>
       </c>
@@ -11275,8 +11920,11 @@
       <c r="L215" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:12">
+      <c r="M215" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13">
       <c r="A216" s="1" t="s">
         <v>140</v>
       </c>
@@ -11314,8 +11962,11 @@
       <c r="L216" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:12">
+      <c r="M216" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13">
       <c r="A217" s="1" t="s">
         <v>140</v>
       </c>
@@ -11353,8 +12004,11 @@
       <c r="L217" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:12">
+      <c r="M217" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13">
       <c r="A218" s="1" t="s">
         <v>140</v>
       </c>
@@ -11392,8 +12046,11 @@
       <c r="L218" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:12">
+      <c r="M218" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13">
       <c r="A219" s="1" t="s">
         <v>140</v>
       </c>
@@ -11431,8 +12088,11 @@
       <c r="L219" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:12">
+      <c r="M219" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13">
       <c r="A220" s="1" t="s">
         <v>140</v>
       </c>
@@ -11470,8 +12130,11 @@
       <c r="L220" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:12">
+      <c r="M220" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13">
       <c r="A221" s="1" t="s">
         <v>140</v>
       </c>
@@ -11507,6 +12170,9 @@
         <v>1</v>
       </c>
       <c r="L221" s="1">
+        <v>0</v>
+      </c>
+      <c r="M221" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sleep pattern mining update
</commit_message>
<xml_diff>
--- a/SlpGroupInfo.xlsx
+++ b/SlpGroupInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="2240" windowWidth="20260" windowHeight="8020"/>
+    <workbookView xWindow="1200" yWindow="2240" windowWidth="20260" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="duration" sheetId="1" r:id="rId1"/>
@@ -1861,11 +1861,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2120770328"/>
-        <c:axId val="2120779320"/>
+        <c:axId val="2103476392"/>
+        <c:axId val="2101493928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2120770328"/>
+        <c:axId val="2103476392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1908,7 +1908,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120779320"/>
+        <c:crossAx val="2101493928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1916,7 +1916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2120779320"/>
+        <c:axId val="2101493928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1967,7 +1967,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120770328"/>
+        <c:crossAx val="2103476392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2883,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G217" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="E214" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2959,7 +2959,7 @@
         <v>7.5211110000000003</v>
       </c>
       <c r="H2">
-        <f>IF(G2&gt;8,IF(G2&gt;9,2,1),0)</f>
+        <f>IF(G2&gt;=8.35,1,0)</f>
         <v>0</v>
       </c>
       <c r="I2" s="1">
@@ -3001,7 +3001,7 @@
         <v>7.71</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="0">IF(G3&gt;8,IF(G3&gt;9,2,1),0)</f>
+        <f t="shared" ref="H3:H66" si="0">IF(G3&gt;=8.35,1,0)</f>
         <v>0</v>
       </c>
       <c r="I3" s="1">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
@@ -3464,7 +3464,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1">
         <v>1</v>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
@@ -3590,7 +3590,7 @@
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="1">
         <v>1</v>
@@ -3674,7 +3674,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1">
         <v>1</v>
@@ -3800,7 +3800,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -4010,7 +4010,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1">
         <v>1</v>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="1">
         <v>1</v>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="1">
         <v>1</v>
@@ -4430,7 +4430,7 @@
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I37" s="1">
         <v>1</v>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" s="1">
         <v>1</v>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="H39">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="1">
         <v>1</v>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="H41">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I41" s="1">
         <v>0</v>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="H44">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="H45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="1">
         <v>1</v>
@@ -4808,7 +4808,7 @@
       </c>
       <c r="H46">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I46" s="1">
         <v>0</v>
@@ -4892,7 +4892,7 @@
       </c>
       <c r="H48">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48" s="1">
         <v>0</v>
@@ -4934,7 +4934,7 @@
       </c>
       <c r="H49">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" s="1">
         <v>0</v>
@@ -5060,7 +5060,7 @@
       </c>
       <c r="H52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
@@ -5102,7 +5102,7 @@
       </c>
       <c r="H53">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53" s="1">
         <v>0</v>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="H54">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54" s="1">
         <v>1</v>
@@ -5186,7 +5186,7 @@
       </c>
       <c r="H55">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="1">
         <v>1</v>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="H56">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" s="1">
         <v>1</v>
@@ -5270,7 +5270,7 @@
       </c>
       <c r="H57">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" s="1">
         <v>1</v>
@@ -5312,7 +5312,7 @@
       </c>
       <c r="H58">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58" s="1">
         <v>0</v>
@@ -5354,7 +5354,7 @@
       </c>
       <c r="H59">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" s="1">
         <v>1</v>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="H64">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" s="1">
         <v>1</v>
@@ -5689,7 +5689,7 @@
         <v>7.2722220000000002</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H130" si="1">IF(G67&gt;8,IF(G67&gt;9,2,1),0)</f>
+        <f t="shared" ref="H67:H130" si="1">IF(G67&gt;=8.35,1,0)</f>
         <v>0</v>
       </c>
       <c r="I67" s="1">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="H68">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68" s="1">
         <v>1</v>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="H69">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" s="1">
         <v>1</v>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="H71">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" s="1">
         <v>1</v>
@@ -5942,7 +5942,7 @@
       </c>
       <c r="H73">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I73" s="1">
         <v>1</v>
@@ -6026,7 +6026,7 @@
       </c>
       <c r="H75">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" s="1">
         <v>1</v>
@@ -6068,7 +6068,7 @@
       </c>
       <c r="H76">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I76" s="1">
         <v>0</v>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="H77">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I77" s="1">
         <v>0</v>
@@ -6488,7 +6488,7 @@
       </c>
       <c r="H86">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I86" s="1">
         <v>1</v>
@@ -6782,7 +6782,7 @@
       </c>
       <c r="H93">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" s="1">
         <v>1</v>
@@ -6908,7 +6908,7 @@
       </c>
       <c r="H96">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" s="1">
         <v>0</v>
@@ -6950,7 +6950,7 @@
       </c>
       <c r="H97">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I97" s="1">
         <v>0</v>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="H98">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I98" s="1">
         <v>0</v>
@@ -7076,7 +7076,7 @@
       </c>
       <c r="H100">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I100" s="1">
         <v>1</v>
@@ -7202,7 +7202,7 @@
       </c>
       <c r="H103">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" s="1">
         <v>0</v>
@@ -7286,7 +7286,7 @@
       </c>
       <c r="H105">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" s="1">
         <v>0</v>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="H111">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I111" s="1">
         <v>0</v>
@@ -7790,7 +7790,7 @@
       </c>
       <c r="H117">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I117" s="1">
         <v>1</v>
@@ -7832,7 +7832,7 @@
       </c>
       <c r="H118">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I118" s="1">
         <v>1</v>
@@ -7958,7 +7958,7 @@
       </c>
       <c r="H121">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I121" s="1">
         <v>0</v>
@@ -8000,7 +8000,7 @@
       </c>
       <c r="H122">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I122" s="1">
         <v>0</v>
@@ -8168,7 +8168,7 @@
       </c>
       <c r="H126">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I126" s="1">
         <v>1</v>
@@ -8377,8 +8377,8 @@
         <v>8.2622219999999995</v>
       </c>
       <c r="H131">
-        <f t="shared" ref="H131:H194" si="2">IF(G131&gt;8,IF(G131&gt;9,2,1),0)</f>
-        <v>1</v>
+        <f t="shared" ref="H131:H194" si="2">IF(G131&gt;=8.35,1,0)</f>
+        <v>0</v>
       </c>
       <c r="I131" s="1">
         <v>1</v>
@@ -8546,7 +8546,7 @@
       </c>
       <c r="H135">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I135" s="1">
         <v>0</v>
@@ -8588,7 +8588,7 @@
       </c>
       <c r="H136">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I136" s="1">
         <v>1</v>
@@ -8756,7 +8756,7 @@
       </c>
       <c r="H140">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I140" s="1">
         <v>1</v>
@@ -8840,7 +8840,7 @@
       </c>
       <c r="H142">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I142" s="1">
         <v>1</v>
@@ -8882,7 +8882,7 @@
       </c>
       <c r="H143">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I143" s="1">
         <v>0</v>
@@ -9050,7 +9050,7 @@
       </c>
       <c r="H147">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I147" s="1">
         <v>0</v>
@@ -9092,7 +9092,7 @@
       </c>
       <c r="H148">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I148" s="1">
         <v>0</v>
@@ -9176,7 +9176,7 @@
       </c>
       <c r="H150">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I150" s="1">
         <v>1</v>
@@ -9302,7 +9302,7 @@
       </c>
       <c r="H153">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I153" s="1">
         <v>0</v>
@@ -9344,7 +9344,7 @@
       </c>
       <c r="H154">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I154" s="1">
         <v>0</v>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="H155">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I155" s="1">
         <v>0</v>
@@ -9554,7 +9554,7 @@
       </c>
       <c r="H159">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I159" s="1">
         <v>0</v>
@@ -9596,7 +9596,7 @@
       </c>
       <c r="H160">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I160" s="1">
         <v>0</v>
@@ -9638,7 +9638,7 @@
       </c>
       <c r="H161">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I161" s="1">
         <v>0</v>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="H162">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I162" s="1">
         <v>1</v>
@@ -9722,7 +9722,7 @@
       </c>
       <c r="H163">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I163" s="1">
         <v>0</v>
@@ -9764,7 +9764,7 @@
       </c>
       <c r="H164">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I164" s="1">
         <v>1</v>
@@ -9932,7 +9932,7 @@
       </c>
       <c r="H168">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I168" s="1">
         <v>1</v>
@@ -10058,7 +10058,7 @@
       </c>
       <c r="H171">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I171" s="1">
         <v>0</v>
@@ -10100,7 +10100,7 @@
       </c>
       <c r="H172">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I172" s="1">
         <v>1</v>
@@ -10226,7 +10226,7 @@
       </c>
       <c r="H175">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I175" s="1">
         <v>0</v>
@@ -10268,7 +10268,7 @@
       </c>
       <c r="H176">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I176" s="1">
         <v>1</v>
@@ -10394,7 +10394,7 @@
       </c>
       <c r="H179">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I179" s="1">
         <v>1</v>
@@ -10478,7 +10478,7 @@
       </c>
       <c r="H181">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I181" s="1">
         <v>1</v>
@@ -10604,7 +10604,7 @@
       </c>
       <c r="H184">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I184" s="1">
         <v>1</v>
@@ -10646,7 +10646,7 @@
       </c>
       <c r="H185">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I185" s="1">
         <v>1</v>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="H186">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I186" s="1">
         <v>1</v>
@@ -10730,7 +10730,7 @@
       </c>
       <c r="H187">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I187" s="1">
         <v>0</v>
@@ -10940,7 +10940,7 @@
       </c>
       <c r="H192">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I192" s="1">
         <v>1</v>
@@ -10982,7 +10982,7 @@
       </c>
       <c r="H193">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I193" s="1">
         <v>0</v>
@@ -11065,8 +11065,8 @@
         <v>8.0222219999999993</v>
       </c>
       <c r="H195">
-        <f t="shared" ref="H195:H221" si="3">IF(G195&gt;8,IF(G195&gt;9,2,1),0)</f>
-        <v>1</v>
+        <f t="shared" ref="H195:H221" si="3">IF(G195&gt;=8.35,1,0)</f>
+        <v>0</v>
       </c>
       <c r="I195" s="1">
         <v>1</v>
@@ -11108,7 +11108,7 @@
       </c>
       <c r="H196">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I196" s="1">
         <v>1</v>
@@ -11234,7 +11234,7 @@
       </c>
       <c r="H199">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I199" s="1">
         <v>1</v>
@@ -11276,7 +11276,7 @@
       </c>
       <c r="H200">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I200" s="1">
         <v>1</v>
@@ -11318,7 +11318,7 @@
       </c>
       <c r="H201">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I201" s="1">
         <v>1</v>
@@ -11360,7 +11360,7 @@
       </c>
       <c r="H202">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I202" s="1">
         <v>1</v>
@@ -11444,7 +11444,7 @@
       </c>
       <c r="H204">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I204" s="1">
         <v>1</v>
@@ -11528,7 +11528,7 @@
       </c>
       <c r="H206">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I206" s="1">
         <v>1</v>
@@ -11654,7 +11654,7 @@
       </c>
       <c r="H209">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I209" s="1">
         <v>0</v>
@@ -11696,7 +11696,7 @@
       </c>
       <c r="H210">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I210" s="1">
         <v>0</v>
@@ -11780,7 +11780,7 @@
       </c>
       <c r="H212">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I212" s="1">
         <v>1</v>
@@ -11864,7 +11864,7 @@
       </c>
       <c r="H214">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I214" s="1">
         <v>1</v>
@@ -12032,7 +12032,7 @@
       </c>
       <c r="H218">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I218" s="1">
         <v>1</v>
@@ -12158,7 +12158,7 @@
       </c>
       <c r="H221">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I221" s="1">
         <v>1</v>

</xml_diff>